<commit_message>
Rewinding to the last functional status until weathermap is integrated
</commit_message>
<xml_diff>
--- a/RAAL/Production/Input/GHI_2024-02-02.xlsx
+++ b/RAAL/Production/Input/GHI_2024-02-02.xlsx
@@ -59,10 +59,10 @@
     <t>+02:00</t>
   </si>
   <si>
-    <t>2024-02-02T07:47:25</t>
-  </si>
-  <si>
-    <t>2024-02-02T17:31:41</t>
+    <t>2024-02-02T07:42:50</t>
+  </si>
+  <si>
+    <t>2024-02-02T17:27:06</t>
   </si>
   <si>
     <t>hour</t>
@@ -472,7 +472,7 @@
         <v>46.073272</v>
       </c>
       <c r="B2">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -487,22 +487,22 @@
         <v>15</v>
       </c>
       <c r="G2">
-        <v>2531.8</v>
+        <v>2531.69</v>
       </c>
       <c r="H2">
-        <v>5706.05</v>
+        <v>5706.12</v>
       </c>
       <c r="I2">
-        <v>669.27</v>
+        <v>668.33</v>
       </c>
       <c r="J2">
-        <v>1848.41</v>
+        <v>743.8099999999999</v>
       </c>
       <c r="K2">
-        <v>1776.3</v>
+        <v>3.05</v>
       </c>
       <c r="L2">
-        <v>1173.14</v>
+        <v>742.86</v>
       </c>
     </row>
   </sheetData>
@@ -564,7 +564,7 @@
         <v>46.073272</v>
       </c>
       <c r="B2">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C2" t="s">
         <v>12</v>
@@ -605,7 +605,7 @@
         <v>46.073272</v>
       </c>
       <c r="B3">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -646,7 +646,7 @@
         <v>46.073272</v>
       </c>
       <c r="B4">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -687,7 +687,7 @@
         <v>46.073272</v>
       </c>
       <c r="B5">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -728,7 +728,7 @@
         <v>46.073272</v>
       </c>
       <c r="B6">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -769,7 +769,7 @@
         <v>46.073272</v>
       </c>
       <c r="B7">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C7" t="s">
         <v>12</v>
@@ -810,7 +810,7 @@
         <v>46.073272</v>
       </c>
       <c r="B8">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -851,7 +851,7 @@
         <v>46.073272</v>
       </c>
       <c r="B9">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -869,22 +869,22 @@
         <v>7</v>
       </c>
       <c r="H9">
-        <v>0.15</v>
+        <v>0.98</v>
       </c>
       <c r="I9">
-        <v>0.89</v>
+        <v>9.039999999999999</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <v>2.52</v>
       </c>
       <c r="K9">
-        <v>0.04</v>
+        <v>0.25</v>
       </c>
       <c r="L9">
         <v>0</v>
       </c>
       <c r="M9">
-        <v>0.04</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="10" spans="1:13">
@@ -892,7 +892,7 @@
         <v>46.073272</v>
       </c>
       <c r="B10">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -910,22 +910,22 @@
         <v>8</v>
       </c>
       <c r="H10">
-        <v>63.38</v>
+        <v>72.91</v>
       </c>
       <c r="I10">
-        <v>312.9</v>
+        <v>343.83</v>
       </c>
       <c r="J10">
-        <v>37.21</v>
+        <v>40.19</v>
       </c>
       <c r="K10">
-        <v>38.05</v>
+        <v>18.23</v>
       </c>
       <c r="L10">
-        <v>30.52</v>
+        <v>0</v>
       </c>
       <c r="M10">
-        <v>33.51</v>
+        <v>18.23</v>
       </c>
     </row>
     <row r="11" spans="1:13">
@@ -933,7 +933,7 @@
         <v>46.073272</v>
       </c>
       <c r="B11">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -951,22 +951,22 @@
         <v>9</v>
       </c>
       <c r="H11">
-        <v>197.36</v>
+        <v>207.46</v>
       </c>
       <c r="I11">
-        <v>579.11</v>
+        <v>591.41</v>
       </c>
       <c r="J11">
-        <v>65.43000000000001</v>
+        <v>66.92</v>
       </c>
       <c r="K11">
-        <v>157.63</v>
+        <v>51.87</v>
       </c>
       <c r="L11">
-        <v>259.5</v>
+        <v>0</v>
       </c>
       <c r="M11">
-        <v>94.58</v>
+        <v>51.87</v>
       </c>
     </row>
     <row r="12" spans="1:13">
@@ -974,7 +974,7 @@
         <v>46.073272</v>
       </c>
       <c r="B12">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -992,22 +992,22 @@
         <v>10</v>
       </c>
       <c r="H12">
-        <v>317.82</v>
+        <v>325.66</v>
       </c>
       <c r="I12">
-        <v>696.46</v>
+        <v>702.51</v>
       </c>
       <c r="J12">
-        <v>80.81</v>
+        <v>81.66</v>
       </c>
       <c r="K12">
-        <v>252.54</v>
+        <v>82.95999999999999</v>
       </c>
       <c r="L12">
-        <v>298.69</v>
+        <v>0</v>
       </c>
       <c r="M12">
-        <v>147.85</v>
+        <v>82.95999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:13">
@@ -1015,7 +1015,7 @@
         <v>46.073272</v>
       </c>
       <c r="B13">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C13" t="s">
         <v>12</v>
@@ -1033,22 +1033,22 @@
         <v>11</v>
       </c>
       <c r="H13">
-        <v>400.85</v>
+        <v>405.29</v>
       </c>
       <c r="I13">
-        <v>753.46</v>
+        <v>756.2</v>
       </c>
       <c r="J13">
-        <v>89.23999999999999</v>
+        <v>89.64</v>
       </c>
       <c r="K13">
-        <v>318.23</v>
+        <v>106.83</v>
       </c>
       <c r="L13">
-        <v>307.54</v>
+        <v>0</v>
       </c>
       <c r="M13">
-        <v>188.1</v>
+        <v>106.83</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -1056,7 +1056,7 @@
         <v>46.073272</v>
       </c>
       <c r="B14">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -1074,22 +1074,22 @@
         <v>12</v>
       </c>
       <c r="H14">
-        <v>435.41</v>
+        <v>435.9</v>
       </c>
       <c r="I14">
-        <v>773.66</v>
+        <v>773.99</v>
       </c>
       <c r="J14">
-        <v>92.40000000000001</v>
+        <v>92.43000000000001</v>
       </c>
       <c r="K14">
-        <v>348.31</v>
+        <v>115.54</v>
       </c>
       <c r="L14">
-        <v>320.5</v>
+        <v>0</v>
       </c>
       <c r="M14">
-        <v>203.24</v>
+        <v>115.54</v>
       </c>
     </row>
     <row r="15" spans="1:13">
@@ -1097,7 +1097,7 @@
         <v>46.073272</v>
       </c>
       <c r="B15">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C15" t="s">
         <v>12</v>
@@ -1115,22 +1115,22 @@
         <v>13</v>
       </c>
       <c r="H15">
-        <v>417.41</v>
+        <v>413.9</v>
       </c>
       <c r="I15">
-        <v>763.41</v>
+        <v>761.39</v>
       </c>
       <c r="J15">
-        <v>90.76000000000001</v>
+        <v>90.43000000000001</v>
       </c>
       <c r="K15">
-        <v>341.42</v>
+        <v>114.53</v>
       </c>
       <c r="L15">
-        <v>342.59</v>
+        <v>0</v>
       </c>
       <c r="M15">
-        <v>191.72</v>
+        <v>114.53</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1138,7 +1138,7 @@
         <v>46.073272</v>
       </c>
       <c r="B16">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
@@ -1156,22 +1156,22 @@
         <v>14</v>
       </c>
       <c r="H16">
-        <v>348.96</v>
+        <v>341.86</v>
       </c>
       <c r="I16">
-        <v>719.55</v>
+        <v>714.51</v>
       </c>
       <c r="J16">
-        <v>84.11</v>
+        <v>83.37</v>
       </c>
       <c r="K16">
-        <v>242.29</v>
+        <v>119.05</v>
       </c>
       <c r="L16">
-        <v>190.91</v>
+        <v>0.63</v>
       </c>
       <c r="M16">
-        <v>167.37</v>
+        <v>118.84</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -1179,7 +1179,7 @@
         <v>46.073272</v>
       </c>
       <c r="B17">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -1197,22 +1197,22 @@
         <v>15</v>
       </c>
       <c r="H17">
-        <v>238.69</v>
+        <v>228.97</v>
       </c>
       <c r="I17">
-        <v>625.95</v>
+        <v>615.72</v>
       </c>
       <c r="J17">
-        <v>71.26000000000001</v>
+        <v>69.95</v>
       </c>
       <c r="K17">
-        <v>88.34999999999999</v>
+        <v>95.68000000000001</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>2.41</v>
       </c>
       <c r="M17">
-        <v>88.34999999999999</v>
+        <v>94.94</v>
       </c>
     </row>
     <row r="18" spans="1:13">
@@ -1220,7 +1220,7 @@
         <v>46.073272</v>
       </c>
       <c r="B18">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
@@ -1238,22 +1238,22 @@
         <v>16</v>
       </c>
       <c r="H18">
-        <v>104.71</v>
+        <v>94.48999999999999</v>
       </c>
       <c r="I18">
-        <v>426.72</v>
+        <v>402.78</v>
       </c>
       <c r="J18">
-        <v>48.45</v>
+        <v>46.02</v>
       </c>
       <c r="K18">
-        <v>56.01</v>
+        <v>37.15</v>
       </c>
       <c r="L18">
-        <v>26.05</v>
+        <v>0</v>
       </c>
       <c r="M18">
-        <v>52.85</v>
+        <v>37.15</v>
       </c>
     </row>
     <row r="19" spans="1:13">
@@ -1261,7 +1261,7 @@
         <v>46.073272</v>
       </c>
       <c r="B19">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
@@ -1279,22 +1279,22 @@
         <v>17</v>
       </c>
       <c r="H19">
-        <v>7.07</v>
+        <v>4.27</v>
       </c>
       <c r="I19">
-        <v>53.94</v>
+        <v>34.74</v>
       </c>
       <c r="J19">
-        <v>8.609999999999999</v>
+        <v>5.2</v>
       </c>
       <c r="K19">
-        <v>5.53</v>
+        <v>1.72</v>
       </c>
       <c r="L19">
         <v>0</v>
       </c>
       <c r="M19">
-        <v>5.53</v>
+        <v>1.72</v>
       </c>
     </row>
     <row r="20" spans="1:13">
@@ -1302,7 +1302,7 @@
         <v>46.073272</v>
       </c>
       <c r="B20">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
@@ -1343,7 +1343,7 @@
         <v>46.073272</v>
       </c>
       <c r="B21">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
@@ -1384,7 +1384,7 @@
         <v>46.073272</v>
       </c>
       <c r="B22">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
@@ -1425,7 +1425,7 @@
         <v>46.073272</v>
       </c>
       <c r="B23">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -1466,7 +1466,7 @@
         <v>46.073272</v>
       </c>
       <c r="B24">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -1507,7 +1507,7 @@
         <v>46.073272</v>
       </c>
       <c r="B25">
-        <v>23.580489</v>
+        <v>24.724419</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>

</xml_diff>